<commit_message>
added some more functions, to make it more efficient
</commit_message>
<xml_diff>
--- a/datatest.xlsx
+++ b/datatest.xlsx
@@ -424,7 +424,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>tejascoder035611@gmail.com</t>
+          <t>UpxVBf3Sre</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -436,7 +436,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>tejasranjith035611@gmail.com</t>
+          <t>YIwJSO9I0U</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">

</xml_diff>